<commit_message>
feat: adding scrpt for sams and natue
</commit_message>
<xml_diff>
--- a/outputs/fahorro.xlsx
+++ b/outputs/fahorro.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,32 +434,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>ids</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>image</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>oldprice</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>category</t>
         </is>

</xml_diff>